<commit_message>
updated to include GIRAFE precip
</commit_message>
<xml_diff>
--- a/ECV_time_coverage_perECV.xlsx
+++ b/ECV_time_coverage_perECV.xlsx
@@ -621,7 +621,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-10-11</t>
+          <t>2024-12-13</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2023-05-31</t>
+          <t>2024-02-29</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-09-30</t>
+          <t>2024-11-30</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2023-09-08</t>
+          <t>2023-12-31</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024-06-30</t>
+          <t>2024-09-30</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2024-09-30</t>
+          <t>2024-12-02</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2023-09-08</t>
+          <t>2023-12-31</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">

</xml_diff>

<commit_message>
make sure information from non standard datasets is checked via manifest files
</commit_message>
<xml_diff>
--- a/ECV_time_coverage_perECV.xlsx
+++ b/ECV_time_coverage_perECV.xlsx
@@ -571,7 +571,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-02-29</t>
+          <t>2024-06-30</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2023-10-31</t>
+          <t>2024-06-30</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-12-13</t>
+          <t>2025-01-19</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2023-10-31</t>
+          <t>2024-06-30</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -841,7 +841,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1992-10-13</t>
+          <t>1992-09-26</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-11-30</t>
+          <t>2024-12-31</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2023-12-31</t>
+          <t>2023-06-07</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2024-12-02</t>
+          <t>2025-01-01</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2023-12-31</t>
+          <t>2023-06-07</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">

</xml_diff>